<commit_message>
Update document for ring buffer
</commit_message>
<xml_diff>
--- a/board_utilities/ring_buffer/doc/Ringbuffer.xlsx
+++ b/board_utilities/ring_buffer/doc/Ringbuffer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/congtri/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Documents/02_CODING/01_Repositories/stm32f411_nuc_template/board_utilities/ring_buffer/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBF95C1-AD19-684B-B0D7-34350B3456E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDC7865-9EF6-0D4F-BD34-E20ECCC3C55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14960" xr2:uid="{7F97C667-664D-EA42-B359-450D554FA1D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>w, r</t>
   </si>
@@ -39,10 +39,16 @@
     <t>full</t>
   </si>
   <si>
-    <t>init</t>
-  </si>
-  <si>
     <t>free</t>
+  </si>
+  <si>
+    <t>Part 1</t>
+  </si>
+  <si>
+    <t>Part 2</t>
+  </si>
+  <si>
+    <t>init/Free</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -115,17 +121,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +481,7 @@
   <dimension ref="B3:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +498,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -477,7 +515,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
@@ -517,7 +555,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="J12" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -549,15 +587,19 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7"/>
       <c r="J18" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
@@ -569,6 +611,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B18:C18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>